<commit_message>
adding archetypes for new MULTI_RES
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\SURB_2040_BLN\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCED52B5-5471-4D4E-B012-B0D0BEC993CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2930" windowWidth="19340" windowHeight="16460" tabRatio="785"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId1"/>
     <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Ths_set_C</t>
   </si>
@@ -148,12 +157,15 @@
   </si>
   <si>
     <t>Ev_kWveh</t>
+  </si>
+  <si>
+    <t>MULTI_RES_2040</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -762,9 +774,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="OPbrntBvG5@student.ethz.ch" id="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" userId="S::OPbrntBvG5@student.ethz.ch::4619f5d3-a278-48a2-998f-258564ebce46" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,90 +1038,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D1" dT="2019-08-09T09:30:43.03" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{4995A51A-970E-4858-A3E9-F23AAFC3B2D7}">
-    <text>do not find this in SIA</text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2019-08-13T15:04:41.29" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{59FCE18A-D39A-4487-B53C-3197D510A233}" parentId="{4995A51A-970E-4858-A3E9-F23AAFC3B2D7}">
-    <text>keep the same as old CEA Databases
-!</text>
-  </threadedComment>
-  <threadedComment ref="F14" dT="2019-08-13T15:40:02.18" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{19AF7AA5-1871-49D1-8FCF-02DD9C759BA1}">
-    <text>do not change from old CEA database</text>
-  </threadedComment>
-  <threadedComment ref="G15" dT="2019-08-13T14:54:06.63" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{1E62239D-37F6-4696-B130-748547BDA1A6}">
-    <text>nothing in SIA</text>
-  </threadedComment>
-  <threadedComment ref="G15" dT="2019-08-14T15:42:57.84" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{16CCDA4D-D51F-44AA-95EC-8AE62BEBEB94}" parentId="{1E62239D-37F6-4696-B130-748547BDA1A6}">
-    <text>Keep same as old CEA database
-These are not used anyway for these building typologies</text>
-  </threadedComment>
-  <threadedComment ref="G16" dT="2019-08-13T14:52:59.52" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{CB14F6D7-71C4-4A0D-B956-D1AB18BB535B}">
-    <text>nothing in SIA 2024</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F1" dT="2019-08-08T12:20:45.51" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{2BD16210-01D2-42DE-9F57-124A6EE12ECA}">
-    <text>dont find in SIA</text>
-  </threadedComment>
-  <threadedComment ref="F1" dT="2019-08-13T08:16:02.08" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{6906B04C-56FB-4FF5-BF02-6B67D8F3AD90}" parentId="{2BD16210-01D2-42DE-9F57-124A6EE12ECA}">
-    <text>kept same as old CEA database - no reference available to change these values</text>
-  </threadedComment>
-  <threadedComment ref="G1" dT="2019-08-08T12:23:57.13" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{2ED044A9-C68D-45BD-B13C-0553F43D3768}">
-    <text>dont find in SIA</text>
-  </threadedComment>
-  <threadedComment ref="J1" dT="2019-08-08T12:08:25.79" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{4188EAE4-5F6C-4CB7-96DC-907AA428BC99}">
-    <text>cannot find in SIA</text>
-  </threadedComment>
-  <threadedComment ref="J1" dT="2019-08-13T12:13:58.38" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{F1EF6245-8799-47A6-BCFF-35017E08DD5E}" parentId="{4188EAE4-5F6C-4CB7-96DC-907AA428BC99}">
-    <text>no other source available - keep same as in old CEA database</text>
-  </threadedComment>
-  <threadedComment ref="K1" dT="2019-08-08T12:08:53.23" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{31840D2C-BF6D-496C-92D3-7147ADE02D81}">
-    <text>no reference available - keep same as in old CEA database</text>
-  </threadedComment>
-  <threadedComment ref="A4" dT="2019-08-08T15:02:30.20" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{BA522695-9F5A-4685-BC9C-BB455B175508}">
-    <text>hotelzimmer values used</text>
-  </threadedComment>
-  <threadedComment ref="A5" dT="2019-08-08T15:03:11.08" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{AB79D271-718E-45F1-9D6A-2D1684E778DD}">
-    <text>einzel/gruppenburo values used</text>
-  </threadedComment>
-  <threadedComment ref="A6" dT="2019-08-08T15:03:58.66" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{99BBF83B-3C08-41AC-84FA-45BAB926754C}">
-    <text>fachgeschaft</text>
-  </threadedComment>
-  <threadedComment ref="A7" dT="2019-08-08T15:04:09.18" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{2E89370B-2C8B-441B-8524-4961F9AD1E21}">
-    <text>lebensmittelverkauf = supermarket</text>
-  </threadedComment>
-  <threadedComment ref="A9" dT="2019-08-08T15:05:24.19" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{10829547-C2A4-4E58-B632-CF7EDF7CE835}">
-    <text>grosse arbeit values are used</text>
-  </threadedComment>
-  <threadedComment ref="A10" dT="2019-08-08T15:08:09.77" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{139CF0AD-AE2C-4F6B-9B40-AE63022A2B59}">
-    <text>schulzimmer values</text>
-  </threadedComment>
-  <threadedComment ref="A11" dT="2019-08-08T14:52:31.15" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{EB7016A0-8719-4E80-9845-07E465C0EED2}">
-    <text>do not know which one to take - 3 categories of rooms are available</text>
-  </threadedComment>
-  <threadedComment ref="A11" dT="2019-08-13T12:21:38.00" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{A96F6928-49E1-45C2-8A9F-9831A5C098A7}" parentId="{EB7016A0-8719-4E80-9845-07E465C0EED2}">
-    <text>all values from Bettenzimmer SIA 2024 8.1</text>
-  </threadedComment>
-  <threadedComment ref="F17" dT="2019-08-13T08:16:17.03" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{74014532-D18F-4AA9-A13E-1879A8CF80D5}">
-    <text>same as industrial</text>
-  </threadedComment>
-  <threadedComment ref="A20" dT="2019-08-08T14:58:20.10" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{4A6E4AE9-26FD-441F-92BA-0F9C18F35B56}">
-    <text>Horsaal is taken for this</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,65 +1153,65 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="9">
+        <v>30</v>
+      </c>
+      <c r="C3" s="9">
+        <v>70</v>
+      </c>
+      <c r="D3" s="9">
+        <v>80</v>
+      </c>
+      <c r="E3" s="9">
+        <v>8</v>
+      </c>
+      <c r="F3" s="9">
+        <v>2.7</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>35</v>
+      </c>
+      <c r="J3" s="9">
+        <v>140</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B4" s="9">
         <v>50</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C4" s="7">
         <v>70</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4" s="7">
         <v>80</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E4" s="7">
         <v>8</v>
       </c>
-      <c r="F3" s="7">
-        <v>2.7</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9">
-        <v>40</v>
-      </c>
-      <c r="J3" s="9">
-        <v>160</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0</v>
-      </c>
-      <c r="L3" s="7">
-        <v>0</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9">
-        <v>15</v>
-      </c>
-      <c r="C4" s="9">
-        <v>70</v>
-      </c>
-      <c r="D4" s="9">
-        <v>80</v>
-      </c>
-      <c r="E4" s="9">
-        <v>8</v>
-      </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>2.7</v>
       </c>
       <c r="G4" s="9">
@@ -1308,11 +1240,11 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
+      <c r="A5" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="9">
         <v>70</v>
@@ -1321,10 +1253,10 @@
         <v>80</v>
       </c>
       <c r="E5" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="9">
-        <v>15.9</v>
+        <v>2.7</v>
       </c>
       <c r="G5" s="9">
         <v>0</v>
@@ -1333,10 +1265,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="9">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="J5" s="9">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="K5" s="7">
         <v>0</v>
@@ -1353,10 +1285,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="9">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9">
         <v>70</v>
@@ -1365,115 +1297,115 @@
         <v>80</v>
       </c>
       <c r="E6" s="9">
+        <v>7</v>
+      </c>
+      <c r="F6" s="9">
+        <v>15.9</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>3</v>
+      </c>
+      <c r="J6" s="9">
+        <v>60</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
+        <v>70</v>
+      </c>
+      <c r="D7" s="9">
+        <v>80</v>
+      </c>
+      <c r="E7" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F7" s="9">
         <f>9.3+24</f>
         <v>33.299999999999997</v>
       </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
         <v>2</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J7" s="9">
         <v>30</v>
       </c>
-      <c r="K6" s="7">
-        <v>0</v>
-      </c>
-      <c r="L6" s="7">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B8" s="9">
         <v>8</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C8" s="9">
         <v>70</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D8" s="9">
         <v>80</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E8" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F8" s="9">
         <f>9.3+12</f>
         <v>21.3</v>
       </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
         <v>2</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J8" s="9">
         <v>30</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K8" s="7">
         <v>10</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="9">
-        <v>70</v>
-      </c>
-      <c r="D8" s="9">
-        <v>80</v>
-      </c>
-      <c r="E8" s="9">
-        <v>2</v>
-      </c>
-      <c r="F8" s="9">
-        <v>6.9</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>15</v>
-      </c>
-      <c r="J8" s="9">
-        <v>45</v>
-      </c>
-      <c r="K8" s="7">
-        <v>0</v>
       </c>
       <c r="L8" s="7">
         <v>0</v>
@@ -1487,40 +1419,40 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>70</v>
+      </c>
+      <c r="D9" s="9">
+        <v>80</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9">
+        <v>6.9</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
         <v>15</v>
       </c>
-      <c r="C9" s="9">
-        <v>90</v>
-      </c>
-      <c r="D9" s="9">
-        <v>170</v>
-      </c>
-      <c r="E9" s="9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9">
-        <v>10.8</v>
-      </c>
-      <c r="G9" s="9">
-        <v>16.5</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>3</v>
-      </c>
       <c r="J9" s="9">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="K9" s="7">
         <v>0</v>
       </c>
       <c r="L9" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7">
         <v>0</v>
@@ -1531,40 +1463,40 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="9">
+        <v>15</v>
+      </c>
+      <c r="C10" s="9">
+        <v>90</v>
+      </c>
+      <c r="D10" s="9">
+        <v>170</v>
+      </c>
+      <c r="E10" s="9">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9">
+        <v>10.8</v>
+      </c>
+      <c r="G10" s="9">
+        <v>16.5</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
         <v>3</v>
       </c>
-      <c r="C10" s="9">
-        <v>70</v>
-      </c>
-      <c r="D10" s="9">
-        <v>80</v>
-      </c>
-      <c r="E10" s="9">
-        <v>4</v>
-      </c>
-      <c r="F10" s="9">
-        <v>14</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>2</v>
-      </c>
       <c r="J10" s="9">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K10" s="7">
         <v>0</v>
       </c>
       <c r="L10" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="M10" s="7">
         <v>0</v>
@@ -1575,89 +1507,89 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>70</v>
+      </c>
+      <c r="D11" s="9">
+        <v>80</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
+      <c r="F11" s="9">
+        <v>14</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>2</v>
+      </c>
+      <c r="J11" s="9">
+        <v>30</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B12" s="9">
         <f>15*0.43+3*0.01+5*0.56</f>
         <v>9.2800000000000011</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C12" s="9">
         <v>70</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D12" s="9">
         <v>80</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E12" s="9">
         <f>0.43*4+0.01*7+0.56*20</f>
         <v>12.990000000000002</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F12" s="9">
         <f>0.43*4.5+0.01*15.9+0.56*15.9</f>
         <v>10.998000000000001</v>
       </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
         <f>0.43*60+0.01*0+0.56*0</f>
         <v>25.8</v>
       </c>
-      <c r="J11" s="9">
-        <f>I11*4</f>
+      <c r="J12" s="9">
+        <f>I12*4</f>
         <v>103.2</v>
       </c>
-      <c r="K11" s="7">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7">
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
         <v>16</v>
-      </c>
-      <c r="M11" s="7">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="9">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9">
-        <v>120</v>
-      </c>
-      <c r="D12" s="9">
-        <v>280</v>
-      </c>
-      <c r="E12" s="9">
-        <v>2</v>
-      </c>
-      <c r="F12" s="9">
-        <v>9.9</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>60</v>
-      </c>
-      <c r="J12" s="9">
-        <v>180</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0</v>
-      </c>
-      <c r="L12" s="7">
-        <v>0</v>
       </c>
       <c r="M12" s="7">
         <v>0</v>
@@ -1668,22 +1600,22 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="9">
         <v>10</v>
       </c>
       <c r="C13" s="9">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D13" s="9">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="E13" s="9">
         <v>2</v>
       </c>
       <c r="F13" s="9">
-        <v>11.3</v>
+        <v>9.9</v>
       </c>
       <c r="G13" s="9">
         <v>0</v>
@@ -1692,10 +1624,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="9">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="J13" s="9">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="K13" s="7">
         <v>0</v>
@@ -1712,34 +1644,34 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14" s="9">
         <v>70</v>
       </c>
       <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2</v>
       </c>
       <c r="F14" s="9">
-        <v>6.6</v>
+        <v>11.3</v>
       </c>
       <c r="G14" s="9">
         <v>0</v>
       </c>
-      <c r="H14" s="9">
-        <v>100</v>
+      <c r="H14" s="7">
+        <v>0</v>
       </c>
       <c r="I14" s="9">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J14" s="9">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="K14" s="7">
         <v>0</v>
@@ -1756,28 +1688,28 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
       </c>
       <c r="C15" s="9">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D15" s="9">
         <v>0</v>
       </c>
-      <c r="E15" s="9">
-        <v>1</v>
+      <c r="E15" s="8">
+        <v>0</v>
       </c>
       <c r="F15" s="9">
-        <v>2.9</v>
+        <v>6.6</v>
       </c>
       <c r="G15" s="9">
         <v>0</v>
       </c>
-      <c r="H15" s="7">
-        <v>0</v>
+      <c r="H15" s="9">
+        <v>100</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
@@ -1800,22 +1732,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="9">
         <v>0</v>
       </c>
       <c r="C16" s="9">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="D16" s="9">
         <v>0</v>
       </c>
       <c r="E16" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="9">
-        <v>5.7</v>
+        <v>2.9</v>
       </c>
       <c r="G16" s="9">
         <v>0</v>
@@ -1830,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L16" s="7">
         <v>0</v>
@@ -1844,40 +1776,37 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B17" s="9">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C17" s="9">
-        <f>C11</f>
         <v>70</v>
       </c>
       <c r="D17" s="9">
-        <f>D11</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E17" s="9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F17" s="9">
-        <v>16.2</v>
+        <v>5.7</v>
       </c>
       <c r="G17" s="9">
-        <f>G9</f>
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="H17" s="7">
         <v>0</v>
       </c>
       <c r="I17" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J17" s="9">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K17" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L17" s="7">
         <v>0</v>
@@ -1891,34 +1820,37 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="9">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9">
+        <f>C12</f>
+        <v>70</v>
+      </c>
+      <c r="D18" s="9">
+        <f>D12</f>
+        <v>80</v>
+      </c>
+      <c r="E18" s="9">
+        <v>20</v>
+      </c>
+      <c r="F18" s="9">
+        <v>16.2</v>
+      </c>
+      <c r="G18" s="9">
+        <f>G10</f>
+        <v>16.5</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="9">
         <v>3</v>
       </c>
-      <c r="C18" s="9">
-        <v>70</v>
-      </c>
-      <c r="D18" s="9">
-        <v>80</v>
-      </c>
-      <c r="E18" s="9">
-        <v>7</v>
-      </c>
-      <c r="F18" s="9">
-        <v>10.8</v>
-      </c>
-      <c r="G18" s="9">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0</v>
-      </c>
-      <c r="I18" s="9">
-        <v>2</v>
-      </c>
       <c r="J18" s="9">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K18" s="7">
         <v>0</v>
@@ -1935,10 +1867,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="9">
         <v>70</v>
@@ -1947,22 +1879,22 @@
         <v>80</v>
       </c>
       <c r="E19" s="9">
+        <v>7</v>
+      </c>
+      <c r="F19" s="9">
+        <v>10.8</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
         <v>2</v>
       </c>
-      <c r="F19" s="9">
-        <v>6.9</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0</v>
-      </c>
-      <c r="I19" s="9">
-        <v>0</v>
-      </c>
       <c r="J19" s="9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K19" s="7">
         <v>0</v>
@@ -1979,10 +1911,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C20" s="9">
         <v>70</v>
@@ -1991,33 +1923,77 @@
         <v>80</v>
       </c>
       <c r="E20" s="9">
+        <v>2</v>
+      </c>
+      <c r="F20" s="9">
+        <v>6.9</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="7">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="9">
+        <v>10</v>
+      </c>
+      <c r="C21" s="9">
+        <v>70</v>
+      </c>
+      <c r="D21" s="9">
+        <v>80</v>
+      </c>
+      <c r="E21" s="9">
         <v>4</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F21" s="9">
         <v>12.5</v>
       </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-      <c r="I20" s="9">
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
+      <c r="I21" s="9">
         <v>2</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J21" s="9">
         <v>30</v>
       </c>
-      <c r="K20" s="7">
-        <v>0</v>
-      </c>
-      <c r="L20" s="7">
-        <v>0</v>
-      </c>
-      <c r="M20" s="7">
-        <v>0</v>
-      </c>
-      <c r="N20" s="7">
+      <c r="K21" s="7">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0</v>
+      </c>
+      <c r="N21" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2028,11 +2004,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2103,7 +2079,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2">
         <v>26</v>
@@ -2129,8 +2105,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
+      <c r="A4" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>26</v>
@@ -2142,11 +2118,11 @@
         <v>28</v>
       </c>
       <c r="E4" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" s="7">
-        <f>36/3.6</f>
-        <v>10</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G4" s="7">
         <v>30</v>
@@ -2157,7 +2133,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>26</v>
@@ -2169,7 +2145,7 @@
         <v>28</v>
       </c>
       <c r="E5" s="4">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F5" s="7">
         <f>36/3.6</f>
@@ -2183,14 +2159,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
+      <c r="A6" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>26</v>
       </c>
       <c r="C6" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
         <v>28</v>
@@ -2199,8 +2175,8 @@
         <v>12</v>
       </c>
       <c r="F6" s="7">
-        <f>30/3.6</f>
-        <v>8.3333333333333339</v>
+        <f>36/3.6</f>
+        <v>10</v>
       </c>
       <c r="G6" s="7">
         <v>30</v>
@@ -2211,7 +2187,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>26</v>
@@ -2238,13 +2214,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>26</v>
       </c>
       <c r="C8" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2">
         <v>28</v>
@@ -2253,183 +2229,184 @@
         <v>12</v>
       </c>
       <c r="F8" s="7">
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G8" s="7">
+        <v>30</v>
+      </c>
+      <c r="H8" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4">
+        <v>12</v>
+      </c>
+      <c r="F9" s="7">
         <f>36/3.6</f>
         <v>10</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="7">
         <v>30</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>30</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>18</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>32</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="4">
         <v>12</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="7">
         <f>10*15/3.6</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="7">
         <v>30</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H10" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>26</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>21</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>28</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E11" s="4">
         <v>12</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F11" s="7">
         <f>25/3.6</f>
         <v>6.9444444444444446</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G11" s="7">
         <v>30</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H11" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
         <v>26</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C12" s="4">
         <v>22</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>28</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="4">
         <v>21</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="7">
         <f>36*1000/3600</f>
         <v>10</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G12" s="7">
         <v>30</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
         <v>26</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <v>18</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <v>28</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E13" s="4">
         <v>12</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F13" s="7">
         <f>9*10/3.6</f>
         <v>25</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G13" s="7">
         <v>30</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <v>30</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>24</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <v>32</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E14" s="4">
         <v>12</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="7">
         <f>3.6*10/3.6</f>
         <v>10</v>
       </c>
-      <c r="G13" s="7">
-        <v>30</v>
-      </c>
-      <c r="H13" s="7">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2">
-        <v>28</v>
-      </c>
-      <c r="E14" s="4">
-        <v>12</v>
-      </c>
-      <c r="F14" s="7">
-        <v>36</v>
-      </c>
       <c r="G14" s="7">
         <v>30</v>
       </c>
       <c r="H14" s="7">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4">
         <v>18</v>
@@ -2441,30 +2418,30 @@
         <v>12</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G15" s="7">
         <v>30</v>
       </c>
       <c r="H15" s="7">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4">
         <v>18</v>
       </c>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4">
-        <v>-18</v>
+        <v>12</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -2478,51 +2455,50 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>-18</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>30</v>
+      </c>
+      <c r="H17" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="2">
         <v>26</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C18" s="4">
         <v>21</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>28</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E18" s="4">
         <v>12</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F18" s="7">
         <f>20*15/3.6</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="G17" s="7">
-        <v>30</v>
-      </c>
-      <c r="H17" s="7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="2">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2">
-        <v>28</v>
-      </c>
-      <c r="E18" s="4">
-        <v>12</v>
-      </c>
-      <c r="F18" s="7">
-        <f>36/3.6</f>
-        <v>10</v>
-      </c>
       <c r="G18" s="7">
         <v>30</v>
       </c>
@@ -2532,7 +2508,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
         <v>26</v>
@@ -2551,7 +2527,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H19" s="7">
         <v>60</v>
@@ -2559,7 +2535,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2">
         <v>26</v>
@@ -2574,13 +2550,40 @@
         <v>12</v>
       </c>
       <c r="F20" s="7">
+        <f>36/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G20" s="7">
+        <v>40</v>
+      </c>
+      <c r="H20" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4">
+        <v>21</v>
+      </c>
+      <c r="D21" s="2">
+        <v>28</v>
+      </c>
+      <c r="E21" s="4">
+        <v>12</v>
+      </c>
+      <c r="F21" s="7">
         <f>30/3.6</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G21" s="7">
         <v>30</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H21" s="7">
         <v>60</v>
       </c>
     </row>
@@ -2588,18 +2591,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F2:F20" unlockedFormula="1"/>
+    <ignoredError sqref="F4:F21 F2" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2769,6 +2766,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2779,22 +2782,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2812,6 +2799,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update setpoints in USE_TYPE_PROPERTIES
Increased Cooling setpoint by 1C
Decreased Heating setpoint by 1C

EXCEPT in Hospital and Coolroom
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\SURB_2040_BLN\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoraiopoulos\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\SURB_2040_BAU\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCED52B5-5471-4D4E-B012-B0D0BEC993CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124C3A4A-B7DB-4103-A807-1B79391A082A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId1"/>
@@ -773,10 +773,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1046,24 +1042,24 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -1107,7 +1103,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1151,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -1195,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1239,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1283,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1327,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1417,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1461,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1505,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1549,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1598,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1642,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1686,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1730,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1774,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -1818,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1865,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1909,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1953,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
@@ -2007,24 +2003,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -2050,15 +2046,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2">
         <v>28</v>
@@ -2077,15 +2073,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2">
         <v>28</v>
@@ -2104,15 +2100,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2">
         <v>28</v>
@@ -2131,15 +2127,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>28</v>
@@ -2158,15 +2154,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2">
         <v>28</v>
@@ -2185,15 +2181,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2">
         <v>28</v>
@@ -2212,15 +2208,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2">
         <v>28</v>
@@ -2239,15 +2235,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2">
         <v>28</v>
@@ -2266,15 +2262,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2">
         <v>32</v>
@@ -2293,15 +2289,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2">
         <v>28</v>
@@ -2320,7 +2316,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -2347,15 +2343,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2">
         <v>28</v>
@@ -2374,15 +2370,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2">
         <v>32</v>
@@ -2401,15 +2397,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2">
         <v>28</v>
@@ -2427,15 +2423,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2">
         <v>28</v>
@@ -2453,7 +2449,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -2479,15 +2475,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2">
         <v>28</v>
@@ -2506,15 +2502,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="2">
         <v>28</v>
@@ -2533,15 +2529,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="2">
         <v>28</v>
@@ -2560,15 +2556,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="2">
         <v>28</v>
@@ -2597,6 +2593,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2766,35 +2777,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2816,9 +2802,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update column names for USE_TYPE_PROPERTIES.xlsx
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/SURB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\SURB_2040_BAU\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3590D7E-F215-44C1-989C-02AB9A951F3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB44905F-1632-4EF5-93E4-E454BA4FB820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26445" yWindow="2955" windowWidth="21600" windowHeight="10425" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="1" r:id="rId1"/>
@@ -58,10 +58,10 @@
     <t>Ed_Wm2</t>
   </si>
   <si>
-    <t>Vww_lpdp</t>
-  </si>
-  <si>
-    <t>Vw_lpdp</t>
+    <t>Vww_ldp</t>
+  </si>
+  <si>
+    <t>Vw_ldp</t>
   </si>
   <si>
     <t>Qcre_Wm2</t>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,8 +569,8 @@
     <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7265625" style="1" customWidth="1"/>
     <col min="12" max="13" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="1"/>
+    <col min="14" max="15" width="9.1796875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -1517,7 +1517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1531,8 +1531,8 @@
     <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="1"/>
+    <col min="9" max="10" width="9.1796875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1578,8 +1578,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="7">
-        <f>30/3.6</f>
-        <v>8.3333333333333339</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="G2" s="7">
         <v>30</v>

</xml_diff>